<commit_message>
fixed dilution and comparisons
</commit_message>
<xml_diff>
--- a/diluted data.xlsx
+++ b/diluted data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ckwr82_umsystem_edu/Documents/Documents/Research/isotope and REY files/REY/fu-rey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\schoolstuff\fu-rey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE91A081-5044-4E23-99CA-EEA25CE32892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF67AFA-CBD2-4D85-9DFB-222474C9AA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="720" windowWidth="23160" windowHeight="13005" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="750" windowWidth="24330" windowHeight="14820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="146">
   <si>
     <t>Sample</t>
   </si>
@@ -13491,15 +13491,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65872D86-0344-4B51-8753-83CC680CA811}">
-  <dimension ref="A1:AG14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -13543,61 +13543,58 @@
         <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AE1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AF1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -13694,11 +13691,8 @@
       <c r="AF2" t="s">
         <v>52</v>
       </c>
-      <c r="AG2" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -13744,59 +13738,56 @@
       <c r="O3">
         <v>1.0249999999999999</v>
       </c>
-      <c r="P3">
-        <v>1.0640000000000001</v>
+      <c r="Q3">
+        <v>37.811999999999998</v>
       </c>
       <c r="R3">
-        <v>37.811999999999998</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="S3">
-        <v>3.7029999999999998</v>
+        <v>42.875</v>
       </c>
       <c r="T3">
-        <v>42.875</v>
+        <v>0.79700000000000004</v>
       </c>
       <c r="U3">
-        <v>0.79700000000000004</v>
+        <v>2.9590000000000001</v>
       </c>
       <c r="V3">
-        <v>2.9590000000000001</v>
+        <v>0.504</v>
       </c>
       <c r="W3">
-        <v>0.504</v>
+        <v>9.4E-2</v>
       </c>
       <c r="X3">
-        <v>9.4E-2</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="Y3">
-        <v>0.76100000000000001</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="Z3">
-        <v>0.26100000000000001</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AA3">
-        <v>5.2999999999999999E-2</v>
+        <v>0.13</v>
       </c>
       <c r="AB3">
-        <v>0.13</v>
+        <v>0.02</v>
       </c>
       <c r="AC3">
-        <v>0.02</v>
-      </c>
-      <c r="AD3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="AE3" t="s">
-        <v>58</v>
+      <c r="AD3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE3">
+        <v>3.5270000000000001</v>
       </c>
       <c r="AF3">
-        <v>3.5270000000000001</v>
-      </c>
-      <c r="AG3">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -13842,59 +13833,56 @@
       <c r="O4">
         <v>0.32800000000000001</v>
       </c>
-      <c r="P4">
-        <v>0.33500000000000002</v>
+      <c r="Q4">
+        <v>39.228999999999999</v>
       </c>
       <c r="R4">
-        <v>39.228999999999999</v>
+        <v>2.3889999999999998</v>
       </c>
       <c r="S4">
-        <v>2.3889999999999998</v>
+        <v>19.364000000000001</v>
       </c>
       <c r="T4">
-        <v>19.364000000000001</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="U4">
-        <v>0.54300000000000004</v>
+        <v>2.0259999999999998</v>
       </c>
       <c r="V4">
-        <v>2.0259999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="W4">
-        <v>0.39</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="X4">
-        <v>8.5999999999999993E-2</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="Y4">
-        <v>0.45800000000000002</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="Z4">
-        <v>0.23499999999999999</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AA4">
-        <v>4.2000000000000003E-2</v>
+        <v>0.12</v>
       </c>
       <c r="AB4">
-        <v>0.12</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AC4">
-        <v>1.6E-2</v>
-      </c>
-      <c r="AD4">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AE4" t="s">
-        <v>58</v>
+      <c r="AD4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE4">
+        <v>1.617</v>
       </c>
       <c r="AF4">
-        <v>1.617</v>
-      </c>
-      <c r="AG4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -13940,59 +13928,56 @@
       <c r="O5">
         <v>0.52700000000000002</v>
       </c>
-      <c r="P5">
-        <v>0.52900000000000003</v>
+      <c r="Q5">
+        <v>21.532</v>
       </c>
       <c r="R5">
-        <v>21.532</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="S5">
-        <v>0.29699999999999999</v>
+        <v>2.5979999999999999</v>
       </c>
       <c r="T5">
-        <v>2.5979999999999999</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="U5">
-        <v>5.0999999999999997E-2</v>
+        <v>0.217</v>
       </c>
       <c r="V5">
-        <v>0.217</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="W5">
-        <v>3.7999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="X5">
+        <v>3.9E-2</v>
+      </c>
+      <c r="Y5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Z5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA5">
+        <v>0.02</v>
+      </c>
+      <c r="AB5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AC5">
         <v>1.2E-2</v>
       </c>
-      <c r="Y5">
-        <v>3.9E-2</v>
-      </c>
-      <c r="Z5">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="AA5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AB5">
-        <v>0.02</v>
-      </c>
-      <c r="AC5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AD5">
-        <v>1.2E-2</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>58</v>
+      <c r="AD5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5">
+        <v>0.55000000000000004</v>
       </c>
       <c r="AF5">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AG5">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -14038,59 +14023,56 @@
       <c r="O6">
         <v>0.307</v>
       </c>
-      <c r="P6">
-        <v>0.32100000000000001</v>
+      <c r="Q6">
+        <v>32.442</v>
       </c>
       <c r="R6">
-        <v>32.442</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="S6">
-        <v>0.61799999999999999</v>
+        <v>3.633</v>
       </c>
       <c r="T6">
-        <v>3.633</v>
+        <v>0.123</v>
       </c>
       <c r="U6">
-        <v>0.123</v>
+        <v>0.505</v>
       </c>
       <c r="V6">
-        <v>0.505</v>
+        <v>0.1</v>
       </c>
       <c r="W6">
-        <v>0.1</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="X6">
-        <v>2.8000000000000001E-2</v>
+        <v>0.111</v>
       </c>
       <c r="Y6">
-        <v>0.111</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="Z6">
-        <v>8.2000000000000003E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AA6">
-        <v>1.7000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="AB6">
-        <v>4.1000000000000002E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AC6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AD6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AE6" t="s">
-        <v>58</v>
+      <c r="AD6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE6">
+        <v>0.81200000000000006</v>
       </c>
       <c r="AF6">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="AG6">
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -14136,59 +14118,56 @@
       <c r="O7">
         <v>0.45200000000000001</v>
       </c>
-      <c r="P7">
-        <v>0.45300000000000001</v>
+      <c r="Q7">
+        <v>39.979999999999997</v>
       </c>
       <c r="R7">
-        <v>39.979999999999997</v>
+        <v>1.238</v>
       </c>
       <c r="S7">
-        <v>1.238</v>
+        <v>6.476</v>
       </c>
       <c r="T7">
-        <v>6.476</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="U7">
-        <v>0.25700000000000001</v>
+        <v>1.0840000000000001</v>
       </c>
       <c r="V7">
-        <v>1.0840000000000001</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="W7">
-        <v>0.22600000000000001</v>
+        <v>6.3E-2</v>
       </c>
       <c r="X7">
-        <v>6.3E-2</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="Y7">
-        <v>0.34799999999999998</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="Z7">
-        <v>0.20300000000000001</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AA7">
-        <v>4.2000000000000003E-2</v>
+        <v>0.123</v>
       </c>
       <c r="AB7">
-        <v>0.123</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="AC7">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="AD7">
         <v>0.105</v>
       </c>
-      <c r="AE7" t="s">
-        <v>58</v>
+      <c r="AD7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE7">
+        <v>5.9039999999999999</v>
       </c>
       <c r="AF7">
-        <v>5.9039999999999999</v>
-      </c>
-      <c r="AG7">
         <v>0.129</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -14234,59 +14213,56 @@
       <c r="O8">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="P8">
-        <v>6.7000000000000004E-2</v>
+      <c r="Q8">
+        <v>88.093999999999994</v>
       </c>
       <c r="R8">
-        <v>88.093999999999994</v>
+        <v>0.214</v>
       </c>
       <c r="S8">
-        <v>0.214</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="T8">
-        <v>0.30499999999999999</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="U8">
-        <v>4.4999999999999998E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="V8">
-        <v>0.18099999999999999</v>
+        <v>3.9E-2</v>
       </c>
       <c r="W8">
-        <v>3.9E-2</v>
+        <v>0.03</v>
       </c>
       <c r="X8">
-        <v>0.03</v>
+        <v>1.9E-2</v>
       </c>
       <c r="Y8">
-        <v>1.9E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="Z8">
-        <v>2.3E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AA8">
-        <v>6.0000000000000001E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AB8">
-        <v>1.4E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="AC8">
-        <v>2E-3</v>
-      </c>
-      <c r="AD8">
         <v>1.2E-2</v>
       </c>
-      <c r="AE8" t="s">
-        <v>58</v>
+      <c r="AD8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE8">
+        <v>0.77900000000000003</v>
       </c>
       <c r="AF8">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="AG8">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -14332,59 +14308,56 @@
       <c r="O9">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="P9">
-        <v>7.3999999999999996E-2</v>
+      <c r="Q9">
+        <v>597.47900000000004</v>
       </c>
       <c r="R9">
-        <v>597.47900000000004</v>
+        <v>0.126</v>
       </c>
       <c r="S9">
-        <v>0.126</v>
+        <v>0.22</v>
       </c>
       <c r="T9">
-        <v>0.22</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="U9">
-        <v>2.5000000000000001E-2</v>
+        <v>0.105</v>
       </c>
       <c r="V9">
-        <v>0.105</v>
+        <v>0.02</v>
       </c>
       <c r="W9">
-        <v>0.02</v>
+        <v>0.157</v>
       </c>
       <c r="X9">
-        <v>0.157</v>
+        <v>2.3E-2</v>
       </c>
       <c r="Y9">
-        <v>2.3E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="Z9">
-        <v>1.2999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AA9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="AB9">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="AC9">
-        <v>1E-3</v>
-      </c>
-      <c r="AD9">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AE9" t="s">
-        <v>58</v>
+      <c r="AD9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9">
+        <v>0.67700000000000005</v>
       </c>
       <c r="AF9">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="AG9">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -14400,14 +14373,11 @@
       <c r="O10" t="s">
         <v>58</v>
       </c>
-      <c r="P10">
-        <v>1.4259999999999999</v>
-      </c>
-      <c r="AA10">
+      <c r="Z10">
         <v>1.909</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -14423,25 +14393,22 @@
       <c r="O11">
         <v>0.55700000000000005</v>
       </c>
-      <c r="P11">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF11">
+      <c r="Z11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE11">
         <v>1031.7919999999999</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AF11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -14453,19 +14420,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E20DF7-7CC8-494B-8A50-CB200DB7C89B}">
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -14509,67 +14476,64 @@
         <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AE1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AF1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AG1" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="AH1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AI1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -14666,11 +14630,8 @@
       <c r="AF2" t="s">
         <v>141</v>
       </c>
-      <c r="AG2" t="s">
-        <v>141</v>
-      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -14732,85 +14693,81 @@
       </c>
       <c r="P3">
         <f>'Processed Data No Duplicates'!P3/1000</f>
-        <v>1.0640000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <f>'Processed Data No Duplicates'!Q3/1000</f>
-        <v>0</v>
+        <v>3.7811999999999998E-2</v>
       </c>
       <c r="R3">
         <f>'Processed Data No Duplicates'!R3/1000</f>
-        <v>3.7811999999999998E-2</v>
+        <v>3.7029999999999997E-3</v>
       </c>
       <c r="S3">
         <f>'Processed Data No Duplicates'!S3/1000</f>
-        <v>3.7029999999999997E-3</v>
+        <v>4.2875000000000003E-2</v>
       </c>
       <c r="T3">
         <f>'Processed Data No Duplicates'!T3/1000</f>
-        <v>4.2875000000000003E-2</v>
+        <v>7.9700000000000007E-4</v>
       </c>
       <c r="U3">
         <f>'Processed Data No Duplicates'!U3/1000</f>
-        <v>7.9700000000000007E-4</v>
+        <v>2.9590000000000003E-3</v>
       </c>
       <c r="V3">
         <f>'Processed Data No Duplicates'!V3/1000</f>
-        <v>2.9590000000000003E-3</v>
+        <v>5.04E-4</v>
       </c>
       <c r="W3">
         <f>'Processed Data No Duplicates'!W3/1000</f>
-        <v>5.04E-4</v>
+        <v>9.3999999999999994E-5</v>
       </c>
       <c r="X3">
         <f>'Processed Data No Duplicates'!X3/1000</f>
-        <v>9.3999999999999994E-5</v>
+        <v>7.6099999999999996E-4</v>
       </c>
       <c r="Y3">
         <f>'Processed Data No Duplicates'!Y3/1000</f>
-        <v>7.6099999999999996E-4</v>
+        <v>2.61E-4</v>
       </c>
       <c r="Z3">
         <f>'Processed Data No Duplicates'!Z3/1000</f>
-        <v>2.61E-4</v>
+        <v>5.3000000000000001E-5</v>
       </c>
       <c r="AA3">
         <f>'Processed Data No Duplicates'!AA3/1000</f>
-        <v>5.3000000000000001E-5</v>
+        <v>1.3000000000000002E-4</v>
       </c>
       <c r="AB3">
         <f>'Processed Data No Duplicates'!AB3/1000</f>
-        <v>1.3000000000000002E-4</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="AC3">
         <f>'Processed Data No Duplicates'!AC3/1000</f>
-        <v>2.0000000000000002E-5</v>
+        <v>1.01E-4</v>
       </c>
       <c r="AD3">
-        <f>'Processed Data No Duplicates'!AD3/1000</f>
-        <v>1.01E-4</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE3/1000</f>
+        <v>3.5270000000000002E-3</v>
       </c>
       <c r="AF3">
         <f>'Processed Data No Duplicates'!AF3/1000</f>
-        <v>3.5270000000000002E-3</v>
+        <v>1.4000000000000001E-4</v>
       </c>
       <c r="AG3">
-        <f>'Processed Data No Duplicates'!AG3/1000</f>
-        <v>1.4000000000000001E-4</v>
-      </c>
-      <c r="AH3">
         <f>C3/E3</f>
         <v>6.8225887029255113E-3</v>
       </c>
-      <c r="AI3">
-        <f>SUM(B3:AG3)</f>
-        <v>22.156128999999989</v>
+      <c r="AH3">
+        <f>SUM(B3:AF3)</f>
+        <v>22.15506499999999</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -14872,85 +14829,81 @@
       </c>
       <c r="P4">
         <f>'Processed Data No Duplicates'!P4/1000</f>
-        <v>3.3500000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <f>'Processed Data No Duplicates'!Q4/1000</f>
-        <v>0</v>
+        <v>3.9229E-2</v>
       </c>
       <c r="R4">
         <f>'Processed Data No Duplicates'!R4/1000</f>
-        <v>3.9229E-2</v>
+        <v>2.3889999999999996E-3</v>
       </c>
       <c r="S4">
         <f>'Processed Data No Duplicates'!S4/1000</f>
-        <v>2.3889999999999996E-3</v>
+        <v>1.9363999999999999E-2</v>
       </c>
       <c r="T4">
         <f>'Processed Data No Duplicates'!T4/1000</f>
-        <v>1.9363999999999999E-2</v>
+        <v>5.4300000000000008E-4</v>
       </c>
       <c r="U4">
         <f>'Processed Data No Duplicates'!U4/1000</f>
-        <v>5.4300000000000008E-4</v>
+        <v>2.0259999999999996E-3</v>
       </c>
       <c r="V4">
         <f>'Processed Data No Duplicates'!V4/1000</f>
-        <v>2.0259999999999996E-3</v>
+        <v>3.8999999999999999E-4</v>
       </c>
       <c r="W4">
         <f>'Processed Data No Duplicates'!W4/1000</f>
-        <v>3.8999999999999999E-4</v>
+        <v>8.599999999999999E-5</v>
       </c>
       <c r="X4">
         <f>'Processed Data No Duplicates'!X4/1000</f>
-        <v>8.599999999999999E-5</v>
+        <v>4.5800000000000002E-4</v>
       </c>
       <c r="Y4">
         <f>'Processed Data No Duplicates'!Y4/1000</f>
-        <v>4.5800000000000002E-4</v>
+        <v>2.3499999999999999E-4</v>
       </c>
       <c r="Z4">
         <f>'Processed Data No Duplicates'!Z4/1000</f>
-        <v>2.3499999999999999E-4</v>
+        <v>4.2000000000000004E-5</v>
       </c>
       <c r="AA4">
         <f>'Processed Data No Duplicates'!AA4/1000</f>
-        <v>4.2000000000000004E-5</v>
+        <v>1.1999999999999999E-4</v>
       </c>
       <c r="AB4">
         <f>'Processed Data No Duplicates'!AB4/1000</f>
-        <v>1.1999999999999999E-4</v>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="AC4">
         <f>'Processed Data No Duplicates'!AC4/1000</f>
-        <v>1.5999999999999999E-5</v>
+        <v>8.2999999999999998E-5</v>
       </c>
       <c r="AD4">
-        <f>'Processed Data No Duplicates'!AD4/1000</f>
-        <v>8.2999999999999998E-5</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE4/1000</f>
+        <v>1.6169999999999999E-3</v>
       </c>
       <c r="AF4">
         <f>'Processed Data No Duplicates'!AF4/1000</f>
-        <v>1.6169999999999999E-3</v>
+        <v>5.9999999999999995E-5</v>
       </c>
       <c r="AG4">
-        <f>'Processed Data No Duplicates'!AG4/1000</f>
-        <v>5.9999999999999995E-5</v>
+        <f t="shared" ref="AG3:AG9" si="0">C4/E4</f>
+        <v>9.2578345270847556E-3</v>
       </c>
       <c r="AH4">
-        <f t="shared" ref="AH4:AH11" si="0">C4/E4</f>
-        <v>9.2578345270847556E-3</v>
-      </c>
-      <c r="AI4">
-        <f t="shared" ref="AI4:AI9" si="1">SUM(B4:AG4)</f>
-        <v>16.396161999999993</v>
+        <f t="shared" ref="AH4:AH9" si="1">SUM(B4:AF4)</f>
+        <v>16.395826999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -15012,85 +14965,81 @@
       </c>
       <c r="P5">
         <f>'Processed Data No Duplicates'!P5/1000</f>
-        <v>5.2900000000000006E-4</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <f>'Processed Data No Duplicates'!Q5/1000</f>
-        <v>0</v>
+        <v>2.1531999999999999E-2</v>
       </c>
       <c r="R5">
         <f>'Processed Data No Duplicates'!R5/1000</f>
-        <v>2.1531999999999999E-2</v>
+        <v>2.9700000000000001E-4</v>
       </c>
       <c r="S5">
         <f>'Processed Data No Duplicates'!S5/1000</f>
-        <v>2.9700000000000001E-4</v>
+        <v>2.598E-3</v>
       </c>
       <c r="T5">
         <f>'Processed Data No Duplicates'!T5/1000</f>
-        <v>2.598E-3</v>
+        <v>5.1E-5</v>
       </c>
       <c r="U5">
         <f>'Processed Data No Duplicates'!U5/1000</f>
-        <v>5.1E-5</v>
+        <v>2.1699999999999999E-4</v>
       </c>
       <c r="V5">
         <f>'Processed Data No Duplicates'!V5/1000</f>
-        <v>2.1699999999999999E-4</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="W5">
         <f>'Processed Data No Duplicates'!W5/1000</f>
-        <v>3.8000000000000002E-5</v>
+        <v>1.2E-5</v>
       </c>
       <c r="X5">
         <f>'Processed Data No Duplicates'!X5/1000</f>
-        <v>1.2E-5</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="Y5">
         <f>'Processed Data No Duplicates'!Y5/1000</f>
-        <v>3.8999999999999999E-5</v>
+        <v>2.8E-5</v>
       </c>
       <c r="Z5">
         <f>'Processed Data No Duplicates'!Z5/1000</f>
-        <v>2.8E-5</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="AA5">
         <f>'Processed Data No Duplicates'!AA5/1000</f>
-        <v>5.0000000000000004E-6</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="AB5">
         <f>'Processed Data No Duplicates'!AB5/1000</f>
-        <v>2.0000000000000002E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="AC5">
         <f>'Processed Data No Duplicates'!AC5/1000</f>
-        <v>3.0000000000000001E-6</v>
+        <v>1.2E-5</v>
       </c>
       <c r="AD5">
-        <f>'Processed Data No Duplicates'!AD5/1000</f>
-        <v>1.2E-5</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE5/1000</f>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="AF5">
         <f>'Processed Data No Duplicates'!AF5/1000</f>
-        <v>5.5000000000000003E-4</v>
+        <v>2.5999999999999998E-5</v>
       </c>
       <c r="AG5">
-        <f>'Processed Data No Duplicates'!AG5/1000</f>
-        <v>2.5999999999999998E-5</v>
-      </c>
-      <c r="AH5">
         <f t="shared" si="0"/>
         <v>1.1238227952538484E-2</v>
       </c>
-      <c r="AI5">
+      <c r="AH5">
         <f t="shared" si="1"/>
-        <v>31.821783000000003</v>
+        <v>31.821254000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -15152,85 +15101,81 @@
       </c>
       <c r="P6">
         <f>'Processed Data No Duplicates'!P6/1000</f>
-        <v>3.21E-4</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'Processed Data No Duplicates'!Q6/1000</f>
-        <v>0</v>
+        <v>3.2441999999999999E-2</v>
       </c>
       <c r="R6">
         <f>'Processed Data No Duplicates'!R6/1000</f>
-        <v>3.2441999999999999E-2</v>
+        <v>6.1799999999999995E-4</v>
       </c>
       <c r="S6">
         <f>'Processed Data No Duplicates'!S6/1000</f>
-        <v>6.1799999999999995E-4</v>
+        <v>3.6329999999999999E-3</v>
       </c>
       <c r="T6">
         <f>'Processed Data No Duplicates'!T6/1000</f>
-        <v>3.6329999999999999E-3</v>
+        <v>1.2300000000000001E-4</v>
       </c>
       <c r="U6">
         <f>'Processed Data No Duplicates'!U6/1000</f>
-        <v>1.2300000000000001E-4</v>
+        <v>5.0500000000000002E-4</v>
       </c>
       <c r="V6">
         <f>'Processed Data No Duplicates'!V6/1000</f>
-        <v>5.0500000000000002E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="W6">
         <f>'Processed Data No Duplicates'!W6/1000</f>
-        <v>1E-4</v>
+        <v>2.8E-5</v>
       </c>
       <c r="X6">
         <f>'Processed Data No Duplicates'!X6/1000</f>
-        <v>2.8E-5</v>
+        <v>1.11E-4</v>
       </c>
       <c r="Y6">
         <f>'Processed Data No Duplicates'!Y6/1000</f>
-        <v>1.11E-4</v>
+        <v>8.2000000000000001E-5</v>
       </c>
       <c r="Z6">
         <f>'Processed Data No Duplicates'!Z6/1000</f>
-        <v>8.2000000000000001E-5</v>
+        <v>1.7E-5</v>
       </c>
       <c r="AA6">
         <f>'Processed Data No Duplicates'!AA6/1000</f>
-        <v>1.7E-5</v>
+        <v>4.1E-5</v>
       </c>
       <c r="AB6">
         <f>'Processed Data No Duplicates'!AB6/1000</f>
-        <v>4.1E-5</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="AC6">
         <f>'Processed Data No Duplicates'!AC6/1000</f>
-        <v>5.0000000000000004E-6</v>
+        <v>3.5000000000000004E-5</v>
       </c>
       <c r="AD6">
-        <f>'Processed Data No Duplicates'!AD6/1000</f>
-        <v>3.5000000000000004E-5</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE6/1000</f>
+        <v>8.12E-4</v>
       </c>
       <c r="AF6">
         <f>'Processed Data No Duplicates'!AF6/1000</f>
-        <v>8.12E-4</v>
+        <v>4.9000000000000005E-5</v>
       </c>
       <c r="AG6">
-        <f>'Processed Data No Duplicates'!AG6/1000</f>
-        <v>4.9000000000000005E-5</v>
-      </c>
-      <c r="AH6">
         <f t="shared" si="0"/>
         <v>8.7726199672818958E-3</v>
       </c>
-      <c r="AI6">
+      <c r="AH6">
         <f t="shared" si="1"/>
-        <v>19.556802999999999</v>
+        <v>19.556481999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -15292,85 +15237,81 @@
       </c>
       <c r="P7">
         <f>'Processed Data No Duplicates'!P7/1000</f>
-        <v>4.5300000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <f>'Processed Data No Duplicates'!Q7/1000</f>
-        <v>0</v>
+        <v>3.9979999999999995E-2</v>
       </c>
       <c r="R7">
         <f>'Processed Data No Duplicates'!R7/1000</f>
-        <v>3.9979999999999995E-2</v>
+        <v>1.238E-3</v>
       </c>
       <c r="S7">
         <f>'Processed Data No Duplicates'!S7/1000</f>
-        <v>1.238E-3</v>
+        <v>6.476E-3</v>
       </c>
       <c r="T7">
         <f>'Processed Data No Duplicates'!T7/1000</f>
-        <v>6.476E-3</v>
+        <v>2.5700000000000001E-4</v>
       </c>
       <c r="U7">
         <f>'Processed Data No Duplicates'!U7/1000</f>
-        <v>2.5700000000000001E-4</v>
+        <v>1.0840000000000001E-3</v>
       </c>
       <c r="V7">
         <f>'Processed Data No Duplicates'!V7/1000</f>
-        <v>1.0840000000000001E-3</v>
+        <v>2.2600000000000002E-4</v>
       </c>
       <c r="W7">
         <f>'Processed Data No Duplicates'!W7/1000</f>
-        <v>2.2600000000000002E-4</v>
+        <v>6.3E-5</v>
       </c>
       <c r="X7">
         <f>'Processed Data No Duplicates'!X7/1000</f>
-        <v>6.3E-5</v>
+        <v>3.48E-4</v>
       </c>
       <c r="Y7">
         <f>'Processed Data No Duplicates'!Y7/1000</f>
-        <v>3.48E-4</v>
+        <v>2.03E-4</v>
       </c>
       <c r="Z7">
         <f>'Processed Data No Duplicates'!Z7/1000</f>
-        <v>2.03E-4</v>
+        <v>4.2000000000000004E-5</v>
       </c>
       <c r="AA7">
         <f>'Processed Data No Duplicates'!AA7/1000</f>
-        <v>4.2000000000000004E-5</v>
+        <v>1.2300000000000001E-4</v>
       </c>
       <c r="AB7">
         <f>'Processed Data No Duplicates'!AB7/1000</f>
-        <v>1.2300000000000001E-4</v>
+        <v>1.7999999999999997E-5</v>
       </c>
       <c r="AC7">
         <f>'Processed Data No Duplicates'!AC7/1000</f>
-        <v>1.7999999999999997E-5</v>
+        <v>1.0499999999999999E-4</v>
       </c>
       <c r="AD7">
-        <f>'Processed Data No Duplicates'!AD7/1000</f>
-        <v>1.0499999999999999E-4</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE7/1000</f>
+        <v>5.9039999999999995E-3</v>
       </c>
       <c r="AF7">
         <f>'Processed Data No Duplicates'!AF7/1000</f>
-        <v>5.9039999999999995E-3</v>
+        <v>1.2899999999999999E-4</v>
       </c>
       <c r="AG7">
-        <f>'Processed Data No Duplicates'!AG7/1000</f>
-        <v>1.2899999999999999E-4</v>
-      </c>
-      <c r="AH7">
         <f t="shared" si="0"/>
         <v>1.2953473515379701E-2</v>
       </c>
-      <c r="AI7">
+      <c r="AH7">
         <f t="shared" si="1"/>
-        <v>31.391868000000002</v>
+        <v>31.391415000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -15432,85 +15373,81 @@
       </c>
       <c r="P8">
         <f>'Processed Data No Duplicates'!P8/1000</f>
-        <v>6.7000000000000002E-5</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <f>'Processed Data No Duplicates'!Q8/1000</f>
-        <v>0</v>
+        <v>8.8093999999999992E-2</v>
       </c>
       <c r="R8">
         <f>'Processed Data No Duplicates'!R8/1000</f>
-        <v>8.8093999999999992E-2</v>
+        <v>2.14E-4</v>
       </c>
       <c r="S8">
         <f>'Processed Data No Duplicates'!S8/1000</f>
-        <v>2.14E-4</v>
+        <v>3.0499999999999999E-4</v>
       </c>
       <c r="T8">
         <f>'Processed Data No Duplicates'!T8/1000</f>
-        <v>3.0499999999999999E-4</v>
+        <v>4.4999999999999996E-5</v>
       </c>
       <c r="U8">
         <f>'Processed Data No Duplicates'!U8/1000</f>
-        <v>4.4999999999999996E-5</v>
+        <v>1.8099999999999998E-4</v>
       </c>
       <c r="V8">
         <f>'Processed Data No Duplicates'!V8/1000</f>
-        <v>1.8099999999999998E-4</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="W8">
         <f>'Processed Data No Duplicates'!W8/1000</f>
-        <v>3.8999999999999999E-5</v>
+        <v>2.9999999999999997E-5</v>
       </c>
       <c r="X8">
         <f>'Processed Data No Duplicates'!X8/1000</f>
-        <v>2.9999999999999997E-5</v>
+        <v>1.9000000000000001E-5</v>
       </c>
       <c r="Y8">
         <f>'Processed Data No Duplicates'!Y8/1000</f>
-        <v>1.9000000000000001E-5</v>
+        <v>2.3E-5</v>
       </c>
       <c r="Z8">
         <f>'Processed Data No Duplicates'!Z8/1000</f>
-        <v>2.3E-5</v>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="AA8">
         <f>'Processed Data No Duplicates'!AA8/1000</f>
-        <v>6.0000000000000002E-6</v>
+        <v>1.4E-5</v>
       </c>
       <c r="AB8">
         <f>'Processed Data No Duplicates'!AB8/1000</f>
-        <v>1.4E-5</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="AC8">
         <f>'Processed Data No Duplicates'!AC8/1000</f>
-        <v>1.9999999999999999E-6</v>
+        <v>1.2E-5</v>
       </c>
       <c r="AD8">
-        <f>'Processed Data No Duplicates'!AD8/1000</f>
-        <v>1.2E-5</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE8/1000</f>
+        <v>7.7900000000000007E-4</v>
       </c>
       <c r="AF8">
         <f>'Processed Data No Duplicates'!AF8/1000</f>
-        <v>7.7900000000000007E-4</v>
+        <v>9.5000000000000005E-5</v>
       </c>
       <c r="AG8">
-        <f>'Processed Data No Duplicates'!AG8/1000</f>
-        <v>9.5000000000000005E-5</v>
-      </c>
-      <c r="AH8">
         <f t="shared" si="0"/>
         <v>1.256524507882621E-2</v>
       </c>
-      <c r="AI8">
+      <c r="AH8">
         <f t="shared" si="1"/>
-        <v>13.922231</v>
+        <v>13.922164000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -15572,85 +15509,81 @@
       </c>
       <c r="P9">
         <f>'Processed Data No Duplicates'!P9/1000</f>
-        <v>7.3999999999999996E-5</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <f>'Processed Data No Duplicates'!Q9/1000</f>
-        <v>0</v>
+        <v>0.59747900000000009</v>
       </c>
       <c r="R9">
         <f>'Processed Data No Duplicates'!R9/1000</f>
-        <v>0.59747900000000009</v>
+        <v>1.26E-4</v>
       </c>
       <c r="S9">
         <f>'Processed Data No Duplicates'!S9/1000</f>
-        <v>1.26E-4</v>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="T9">
         <f>'Processed Data No Duplicates'!T9/1000</f>
-        <v>2.2000000000000001E-4</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="U9">
         <f>'Processed Data No Duplicates'!U9/1000</f>
-        <v>2.5000000000000001E-5</v>
+        <v>1.0499999999999999E-4</v>
       </c>
       <c r="V9">
         <f>'Processed Data No Duplicates'!V9/1000</f>
-        <v>1.0499999999999999E-4</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="W9">
         <f>'Processed Data No Duplicates'!W9/1000</f>
-        <v>2.0000000000000002E-5</v>
+        <v>1.5699999999999999E-4</v>
       </c>
       <c r="X9">
         <f>'Processed Data No Duplicates'!X9/1000</f>
-        <v>1.5699999999999999E-4</v>
+        <v>2.3E-5</v>
       </c>
       <c r="Y9">
         <f>'Processed Data No Duplicates'!Y9/1000</f>
-        <v>2.3E-5</v>
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="Z9">
         <f>'Processed Data No Duplicates'!Z9/1000</f>
-        <v>1.2999999999999999E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="AA9">
         <f>'Processed Data No Duplicates'!AA9/1000</f>
-        <v>3.0000000000000001E-6</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AB9">
         <f>'Processed Data No Duplicates'!AB9/1000</f>
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AC9">
         <f>'Processed Data No Duplicates'!AC9/1000</f>
-        <v>9.9999999999999995E-7</v>
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="AD9">
-        <f>'Processed Data No Duplicates'!AD9/1000</f>
-        <v>6.9999999999999999E-6</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <v>0</v>
+        <f>'Processed Data No Duplicates'!AE9/1000</f>
+        <v>6.7700000000000008E-4</v>
       </c>
       <c r="AF9">
         <f>'Processed Data No Duplicates'!AF9/1000</f>
-        <v>6.7700000000000008E-4</v>
+        <v>5.3999999999999998E-5</v>
       </c>
       <c r="AG9">
-        <f>'Processed Data No Duplicates'!AG9/1000</f>
-        <v>5.3999999999999998E-5</v>
-      </c>
-      <c r="AH9">
         <f t="shared" si="0"/>
         <v>1.3611435488718588E-2</v>
       </c>
-      <c r="AI9">
+      <c r="AH9">
         <f t="shared" si="1"/>
-        <v>9.0491919999999979</v>
+        <v>9.0491179999999982</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -15710,7 +15643,7 @@
       </c>
       <c r="P10">
         <f>'Processed Data No Duplicates'!P10/1000</f>
-        <v>1.426E-3</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <f>'Processed Data No Duplicates'!Q10/1000</f>
@@ -15750,11 +15683,11 @@
       </c>
       <c r="Z10">
         <f>'Processed Data No Duplicates'!Z10/1000</f>
-        <v>0</v>
+        <v>1.9090000000000001E-3</v>
       </c>
       <c r="AA10">
         <f>'Processed Data No Duplicates'!AA10/1000</f>
-        <v>1.9090000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="AB10">
         <f>'Processed Data No Duplicates'!AB10/1000</f>
@@ -15776,12 +15709,8 @@
         <f>'Processed Data No Duplicates'!AF10/1000</f>
         <v>0</v>
       </c>
-      <c r="AG10">
-        <f>'Processed Data No Duplicates'!AG10/1000</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -15842,7 +15771,7 @@
       </c>
       <c r="P11">
         <f>'Processed Data No Duplicates'!P11/1000</f>
-        <v>1.8099999999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <f>'Processed Data No Duplicates'!Q11/1000</f>
@@ -15881,10 +15810,10 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <f>'Processed Data No Duplicates'!Z11/1000</f>
         <v>0</v>
       </c>
       <c r="AA11">
+        <f>'Processed Data No Duplicates'!AA11/1000</f>
         <v>0</v>
       </c>
       <c r="AB11">
@@ -15901,13 +15830,9 @@
       </c>
       <c r="AE11">
         <f>'Processed Data No Duplicates'!AE11/1000</f>
-        <v>0</v>
+        <v>1.0317919999999998</v>
       </c>
       <c r="AF11">
-        <f>'Processed Data No Duplicates'!AF11/1000</f>
-        <v>1.0317919999999998</v>
-      </c>
-      <c r="AG11">
         <v>0</v>
       </c>
     </row>
@@ -15918,10 +15843,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D575FE-4276-4474-AC10-D062BE6C1DA1}">
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15929,7 +15854,7 @@
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -15973,1101 +15898,1061 @@
         <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AB1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AE1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AF1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG1" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>143</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" t="s">
-        <v>141</v>
-      </c>
-      <c r="L2" t="s">
-        <v>141</v>
-      </c>
-      <c r="M2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" t="s">
-        <v>141</v>
-      </c>
-      <c r="P2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S2" t="s">
-        <v>141</v>
-      </c>
-      <c r="T2" t="s">
-        <v>141</v>
-      </c>
-      <c r="U2" t="s">
-        <v>141</v>
-      </c>
-      <c r="V2" t="s">
-        <v>141</v>
-      </c>
-      <c r="W2" t="s">
-        <v>141</v>
-      </c>
-      <c r="X2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>141</v>
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <f>('Formula (ppm)'!B3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>2534.1923395651138</v>
+      </c>
+      <c r="C2">
+        <f>('Formula (ppm)'!C3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>2622.7171654424556</v>
+      </c>
+      <c r="D2">
+        <f>('Formula (ppm)'!D3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>2446.9669606731277</v>
+      </c>
+      <c r="E2">
+        <f>('Formula (ppm)'!E3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>384416.71917256864</v>
+      </c>
+      <c r="F2">
+        <f>('Formula (ppm)'!F3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>20.989678388450148</v>
+      </c>
+      <c r="G2">
+        <f>('Formula (ppm)'!G3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>10.106809886098096</v>
+      </c>
+      <c r="H2">
+        <f>('Formula (ppm)'!H3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>1186.3229061303571</v>
+      </c>
+      <c r="I2">
+        <f>('Formula (ppm)'!I3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>3902.7987811411695</v>
+      </c>
+      <c r="J2">
+        <f>('Formula (ppm)'!J3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>543.00640900541669</v>
+      </c>
+      <c r="K2">
+        <f>('Formula (ppm)'!K3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>212.09862460968714</v>
+      </c>
+      <c r="L2">
+        <f>('Formula (ppm)'!L3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>1.2453033609656583</v>
+      </c>
+      <c r="M2">
+        <f>('Formula (ppm)'!M3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>226.17596695103805</v>
+      </c>
+      <c r="N2">
+        <f>('Formula (ppm)'!N3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>18.246401419366379</v>
+      </c>
+      <c r="O2">
+        <f>('Formula (ppm)'!O3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>18.49907166651883</v>
+      </c>
+      <c r="P2">
+        <f>('Formula (ppm)'!P3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>('Formula (ppm)'!Q3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>682.42624180918062</v>
+      </c>
+      <c r="R2">
+        <f>('Formula (ppm)'!R3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>66.831280371823652</v>
+      </c>
+      <c r="S2">
+        <f>('Formula (ppm)'!S3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>773.80263190438541</v>
+      </c>
+      <c r="T2">
+        <f>('Formula (ppm)'!T3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>14.384156212893181</v>
+      </c>
+      <c r="U2">
+        <f>('Formula (ppm)'!U3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>53.403661523150468</v>
+      </c>
+      <c r="V2">
+        <f>('Formula (ppm)'!V3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>9.0961288974882848</v>
+      </c>
+      <c r="W2">
+        <f>('Formula (ppm)'!W3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>1.6965002308807513</v>
+      </c>
+      <c r="X2">
+        <f>('Formula (ppm)'!X3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>13.734432720215446</v>
+      </c>
+      <c r="Y2">
+        <f>('Formula (ppm)'!Y3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>4.7104953219135766</v>
+      </c>
+      <c r="Z2">
+        <f>('Formula (ppm)'!Z3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>0.95653736421999824</v>
+      </c>
+      <c r="AA2">
+        <f>('Formula (ppm)'!AA3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>2.3462237235584866</v>
+      </c>
+      <c r="AB2">
+        <f>('Formula (ppm)'!AB3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>0.36095749593207482</v>
+      </c>
+      <c r="AC2">
+        <f>('Formula (ppm)'!AC3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>1.8228353544569778</v>
+      </c>
+      <c r="AD2">
+        <f>('Formula (ppm)'!AD3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <f>('Formula (ppm)'!AE3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>63.654854407621393</v>
+      </c>
+      <c r="AF2">
+        <f>('Formula (ppm)'!AF3*(400435-(85475*'Formula (ppm)'!$AG3)))/'Formula (ppm)'!$AH3</f>
+        <v>2.5267024715245241</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B3">
-        <f>('Formula (ppm)'!B3*(400435-(85475*'Formula (ppm)'!AH3)))/'Formula (ppm)'!$AI3</f>
-        <v>2534.0706404790826</v>
+        <f>('Formula (ppm)'!B4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>6301.2550256526974</v>
       </c>
       <c r="C3">
-        <f>('Formula (ppm)'!C3*(400435-(85475*'Formula (ppm)'!AI3)))/'Formula (ppm)'!$AI3</f>
-        <v>-9794.8108873297751</v>
+        <f>('Formula (ppm)'!C4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>3503.5490786730475</v>
       </c>
       <c r="D3">
-        <f>('Formula (ppm)'!D3*(400435-(85475*'Formula (ppm)'!AJ3)))/'Formula (ppm)'!$AI3</f>
-        <v>2450.4180387286974</v>
+        <f>('Formula (ppm)'!D4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>2807.7483314764263</v>
       </c>
       <c r="E3">
-        <f>('Formula (ppm)'!E3*(400435-(85475*'Formula (ppm)'!AK3)))/'Formula (ppm)'!$AI3</f>
-        <v>384958.88101008098</v>
+        <f>('Formula (ppm)'!E4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>378441.53170193866</v>
       </c>
       <c r="F3">
-        <f>('Formula (ppm)'!F3*(400435-(85475*'Formula (ppm)'!AL3)))/'Formula (ppm)'!$AI3</f>
-        <v>21.019281165947362</v>
+        <f>('Formula (ppm)'!F4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>23.277857268015616</v>
       </c>
       <c r="G3">
-        <f>('Formula (ppm)'!G3*(400435-(85475*'Formula (ppm)'!AM3)))/'Formula (ppm)'!$AI3</f>
-        <v>10.121064017997012</v>
+        <f>('Formula (ppm)'!G4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>4.2412012195127931</v>
       </c>
       <c r="H3">
-        <f>('Formula (ppm)'!H3*(400435-(85475*'Formula (ppm)'!AN3)))/'Formula (ppm)'!$AI3</f>
-        <v>1187.9960357696064</v>
+        <f>('Formula (ppm)'!H4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>1746.8874080462235</v>
       </c>
       <c r="I3">
-        <f>('Formula (ppm)'!I3*(400435-(85475*'Formula (ppm)'!AO3)))/'Formula (ppm)'!$AI3</f>
-        <v>3908.3030905353571</v>
+        <f>('Formula (ppm)'!I4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>4503.8144490474533</v>
       </c>
       <c r="J3">
-        <f>('Formula (ppm)'!J3*(400435-(85475*'Formula (ppm)'!AP3)))/'Formula (ppm)'!$AI3</f>
-        <v>543.772237695493</v>
+        <f>('Formula (ppm)'!J4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>58.182455810212851</v>
       </c>
       <c r="K3">
-        <f>('Formula (ppm)'!K3*(400435-(85475*'Formula (ppm)'!AQ3)))/'Formula (ppm)'!$AI3</f>
-        <v>212.39775774910871</v>
+        <f>('Formula (ppm)'!K4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>342.83043191061739</v>
       </c>
       <c r="L3">
-        <f>('Formula (ppm)'!L3*(400435-(85475*'Formula (ppm)'!AR3)))/'Formula (ppm)'!$AI3</f>
-        <v>1.2470596736460604</v>
+        <f>('Formula (ppm)'!L4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>0.63374271096168167</v>
       </c>
       <c r="M3">
-        <f>('Formula (ppm)'!M3*(400435-(85475*'Formula (ppm)'!AS3)))/'Formula (ppm)'!$AI3</f>
-        <v>226.49495405989023</v>
+        <f>('Formula (ppm)'!M4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>252.52209559857778</v>
       </c>
       <c r="N3">
-        <f>('Formula (ppm)'!N3*(400435-(85475*'Formula (ppm)'!AT3)))/'Formula (ppm)'!$AI3</f>
-        <v>18.272135218205321</v>
+        <f>('Formula (ppm)'!N4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>24.447843811329488</v>
       </c>
       <c r="O3">
-        <f>('Formula (ppm)'!O3*(400435-(85475*'Formula (ppm)'!AU3)))/'Formula (ppm)'!$AI3</f>
-        <v>18.525161818655242</v>
+        <f>('Formula (ppm)'!O4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>7.9949080459781383</v>
       </c>
       <c r="P3">
-        <f>('Formula (ppm)'!P3*(400435-(85475*'Formula (ppm)'!AV3)))/'Formula (ppm)'!$AI3</f>
-        <v>19.230021634194323</v>
+        <f>('Formula (ppm)'!P4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f>('Formula (ppm)'!Q3*(400435-(85475*'Formula (ppm)'!AW3)))/'Formula (ppm)'!$AI3</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>956.1958772429158</v>
       </c>
       <c r="R3">
-        <f>('Formula (ppm)'!R3*(400435-(85475*'Formula (ppm)'!AX3)))/'Formula (ppm)'!$AI3</f>
-        <v>683.38870115804104</v>
+        <f>('Formula (ppm)'!R4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>58.231205249517593</v>
       </c>
       <c r="S3">
-        <f>('Formula (ppm)'!S3*(400435-(85475*'Formula (ppm)'!AY3)))/'Formula (ppm)'!$AI3</f>
-        <v>66.925535819005233</v>
+        <f>('Formula (ppm)'!S4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>471.99207134853862</v>
       </c>
       <c r="T3">
-        <f>('Formula (ppm)'!T3*(400435-(85475*'Formula (ppm)'!AZ3)))/'Formula (ppm)'!$AI3</f>
-        <v>774.89396387789634</v>
+        <f>('Formula (ppm)'!T4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>13.2354727712382</v>
       </c>
       <c r="U3">
-        <f>('Formula (ppm)'!U3*(400435-(85475*'Formula (ppm)'!BA3)))/'Formula (ppm)'!$AI3</f>
-        <v>14.404442897042177</v>
+        <f>('Formula (ppm)'!U4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>49.383182015706417</v>
       </c>
       <c r="V3">
-        <f>('Formula (ppm)'!V3*(400435-(85475*'Formula (ppm)'!BB3)))/'Formula (ppm)'!$AI3</f>
-        <v>53.478979337952069</v>
+        <f>('Formula (ppm)'!V4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>9.5061406644252244</v>
       </c>
       <c r="W3">
-        <f>('Formula (ppm)'!W3*(400435-(85475*'Formula (ppm)'!BC3)))/'Formula (ppm)'!$AI3</f>
-        <v>9.1089576161973103</v>
+        <f>('Formula (ppm)'!W4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>2.0962258901040238</v>
       </c>
       <c r="X3">
-        <f>('Formula (ppm)'!X3*(400435-(85475*'Formula (ppm)'!BD3)))/'Formula (ppm)'!$AI3</f>
-        <v>1.6988928887352126</v>
+        <f>('Formula (ppm)'!X4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>11.163621600786547</v>
       </c>
       <c r="Y3">
-        <f>('Formula (ppm)'!Y3*(400435-(85475*'Formula (ppm)'!BE3)))/'Formula (ppm)'!$AI3</f>
-        <v>13.753803067313795</v>
+        <f>('Formula (ppm)'!Y4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>5.7280591183075069</v>
       </c>
       <c r="Z3">
-        <f>('Formula (ppm)'!Z3*(400435-(85475*'Formula (ppm)'!BF3)))/'Formula (ppm)'!$AI3</f>
-        <v>4.7171387655307502</v>
+        <f>('Formula (ppm)'!Z4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>1.0237382253996397</v>
       </c>
       <c r="AA3">
-        <f>('Formula (ppm)'!AA3*(400435-(85475*'Formula (ppm)'!BG3)))/'Formula (ppm)'!$AI3</f>
-        <v>0.95788641598900282</v>
+        <f>('Formula (ppm)'!AA4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>2.9249663582846845</v>
       </c>
       <c r="AB3">
-        <f>('Formula (ppm)'!AB3*(400435-(85475*'Formula (ppm)'!BH3)))/'Formula (ppm)'!$AI3</f>
-        <v>2.3495327184635921</v>
+        <f>('Formula (ppm)'!AB4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>0.38999551443795794</v>
       </c>
       <c r="AC3">
-        <f>('Formula (ppm)'!AC3*(400435-(85475*'Formula (ppm)'!BI3)))/'Formula (ppm)'!$AI3</f>
-        <v>0.36146657207132188</v>
+        <f>('Formula (ppm)'!AC4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>2.0231017311469071</v>
       </c>
       <c r="AD3">
-        <f>('Formula (ppm)'!AD3*(400435-(85475*'Formula (ppm)'!BJ3)))/'Formula (ppm)'!$AI3</f>
-        <v>1.8254061889601754</v>
+        <f>('Formula (ppm)'!AD4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <f>('Formula (ppm)'!AE3*(400435-(85475*'Formula (ppm)'!BK3)))/'Formula (ppm)'!$AI3</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>39.413921677886123</v>
       </c>
       <c r="AF3">
-        <f>('Formula (ppm)'!AF3*(400435-(85475*'Formula (ppm)'!BL3)))/'Formula (ppm)'!$AI3</f>
-        <v>63.744629984777603</v>
-      </c>
-      <c r="AG3">
-        <f>('Formula (ppm)'!AG3*(400435-(85475*'Formula (ppm)'!BM3)))/'Formula (ppm)'!$AI3</f>
-        <v>2.5302660044992531</v>
+        <f>('Formula (ppm)'!AF4*(400435-(85475*'Formula (ppm)'!$AG4)))/'Formula (ppm)'!$AH4</f>
+        <v>1.4624831791423423</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4">
-        <f>('Formula (ppm)'!B4*(400435-(85475*'Formula (ppm)'!AH4)))/'Formula (ppm)'!$AI4</f>
-        <v>6301.1262808626916</v>
+        <f>('Formula (ppm)'!B5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>7716.6200654494478</v>
       </c>
       <c r="C4">
-        <f>('Formula (ppm)'!C4*(400435-(85475*'Formula (ppm)'!AI4)))/'Formula (ppm)'!$AI4</f>
-        <v>-8775.5055282908343</v>
+        <f>('Formula (ppm)'!C5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>4311.5048071110532</v>
       </c>
       <c r="D4">
-        <f>('Formula (ppm)'!D4*(400435-(85475*'Formula (ppm)'!AJ4)))/'Formula (ppm)'!$AI4</f>
-        <v>2813.2503255944912</v>
+        <f>('Formula (ppm)'!D5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>1447.6422377289468</v>
       </c>
       <c r="E4">
-        <f>('Formula (ppm)'!E4*(400435-(85475*'Formula (ppm)'!AK4)))/'Formula (ppm)'!$AI4</f>
-        <v>379183.11635826743</v>
+        <f>('Formula (ppm)'!E5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>383646.32087189273</v>
       </c>
       <c r="F4">
-        <f>('Formula (ppm)'!F4*(400435-(85475*'Formula (ppm)'!AL4)))/'Formula (ppm)'!$AI4</f>
-        <v>23.323471980820887</v>
+        <f>('Formula (ppm)'!F5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.41427203375988803</v>
       </c>
       <c r="G4">
-        <f>('Formula (ppm)'!G4*(400435-(85475*'Formula (ppm)'!AM4)))/'Formula (ppm)'!$AI4</f>
-        <v>4.2495121724218166</v>
+        <f>('Formula (ppm)'!G5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>2.0336990748212687</v>
       </c>
       <c r="H4">
-        <f>('Formula (ppm)'!H4*(400435-(85475*'Formula (ppm)'!AN4)))/'Formula (ppm)'!$AI4</f>
-        <v>1750.3105653627974</v>
+        <f>('Formula (ppm)'!H5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>270.44431585725056</v>
       </c>
       <c r="I4">
-        <f>('Formula (ppm)'!I4*(400435-(85475*'Formula (ppm)'!AO4)))/'Formula (ppm)'!$AI4</f>
-        <v>4512.6400123394751</v>
+        <f>('Formula (ppm)'!I5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>1295.5290791511115</v>
       </c>
       <c r="J4">
-        <f>('Formula (ppm)'!J4*(400435-(85475*'Formula (ppm)'!AP4)))/'Formula (ppm)'!$AI4</f>
-        <v>58.296468710177436</v>
+        <f>('Formula (ppm)'!J5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>49.022190661586748</v>
       </c>
       <c r="K4">
-        <f>('Formula (ppm)'!K4*(400435-(85475*'Formula (ppm)'!AQ4)))/'Formula (ppm)'!$AI4</f>
-        <v>343.50223393743011</v>
+        <f>('Formula (ppm)'!K5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>92.884811448163987</v>
       </c>
       <c r="L4">
-        <f>('Formula (ppm)'!L4*(400435-(85475*'Formula (ppm)'!AR4)))/'Formula (ppm)'!$AI4</f>
-        <v>0.63498457748831727</v>
+        <f>('Formula (ppm)'!L5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>1.569212249090485</v>
       </c>
       <c r="M4">
-        <f>('Formula (ppm)'!M4*(400435-(85475*'Formula (ppm)'!AS4)))/'Formula (ppm)'!$AI4</f>
-        <v>253.0169316453449</v>
+        <f>('Formula (ppm)'!M5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>312.52431152886095</v>
       </c>
       <c r="N4">
-        <f>('Formula (ppm)'!N4*(400435-(85475*'Formula (ppm)'!AT4)))/'Formula (ppm)'!$AI4</f>
-        <v>24.495751200799319</v>
+        <f>('Formula (ppm)'!N5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>2.0713601687994401</v>
       </c>
       <c r="O4">
-        <f>('Formula (ppm)'!O4*(400435-(85475*'Formula (ppm)'!AU4)))/'Formula (ppm)'!$AI4</f>
-        <v>8.0105746698526197</v>
+        <f>('Formula (ppm)'!O5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>6.6157988421654847</v>
       </c>
       <c r="P4">
-        <f>('Formula (ppm)'!P4*(400435-(85475*'Formula (ppm)'!AV4)))/'Formula (ppm)'!$AI4</f>
-        <v>8.1815320560994742</v>
+        <f>('Formula (ppm)'!P5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <f>('Formula (ppm)'!Q4*(400435-(85475*'Formula (ppm)'!AW4)))/'Formula (ppm)'!$AI4</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>270.30622517933057</v>
       </c>
       <c r="R4">
-        <f>('Formula (ppm)'!R4*(400435-(85475*'Formula (ppm)'!AX4)))/'Formula (ppm)'!$AI4</f>
-        <v>958.06961501112312</v>
+        <f>('Formula (ppm)'!R5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>3.728448303838992</v>
       </c>
       <c r="S4">
-        <f>('Formula (ppm)'!S4*(400435-(85475*'Formula (ppm)'!AY4)))/'Formula (ppm)'!$AI4</f>
-        <v>58.345313677676529</v>
+        <f>('Formula (ppm)'!S5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>32.614507385096637</v>
       </c>
       <c r="T4">
-        <f>('Formula (ppm)'!T4*(400435-(85475*'Formula (ppm)'!AZ4)))/'Formula (ppm)'!$AI4</f>
-        <v>472.91697532629911</v>
+        <f>('Formula (ppm)'!T5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.64023859762891777</v>
       </c>
       <c r="U4">
-        <f>('Formula (ppm)'!U4*(400435-(85475*'Formula (ppm)'!BA4)))/'Formula (ppm)'!$AI4</f>
-        <v>13.261408676006013</v>
+        <f>('Formula (ppm)'!U5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>2.7241524644210817</v>
       </c>
       <c r="V4">
-        <f>('Formula (ppm)'!V4*(400435-(85475*'Formula (ppm)'!BB4)))/'Formula (ppm)'!$AI4</f>
-        <v>49.47995207658964</v>
+        <f>('Formula (ppm)'!V5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.47704052372350747</v>
       </c>
       <c r="W4">
-        <f>('Formula (ppm)'!W4*(400435-(85475*'Formula (ppm)'!BC4)))/'Formula (ppm)'!$AI4</f>
-        <v>9.5247686623247603</v>
+        <f>('Formula (ppm)'!W5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.15064437591268656</v>
       </c>
       <c r="X4">
-        <f>('Formula (ppm)'!X4*(400435-(85475*'Formula (ppm)'!BD4)))/'Formula (ppm)'!$AI4</f>
-        <v>2.1003336024613568</v>
+        <f>('Formula (ppm)'!X5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.48959422171623129</v>
       </c>
       <c r="Y4">
-        <f>('Formula (ppm)'!Y4*(400435-(85475*'Formula (ppm)'!BE4)))/'Formula (ppm)'!$AI4</f>
-        <v>11.185497557294207</v>
+        <f>('Formula (ppm)'!Y5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.35150354379626864</v>
       </c>
       <c r="Z4">
-        <f>('Formula (ppm)'!Z4*(400435-(85475*'Formula (ppm)'!BF4)))/'Formula (ppm)'!$AI4</f>
-        <v>5.739283681144407</v>
+        <f>('Formula (ppm)'!Z5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>6.2768489963619403E-2</v>
       </c>
       <c r="AA4">
-        <f>('Formula (ppm)'!AA4*(400435-(85475*'Formula (ppm)'!BG4)))/'Formula (ppm)'!$AI4</f>
-        <v>1.025744317481128</v>
+        <f>('Formula (ppm)'!AA5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.25107395985447761</v>
       </c>
       <c r="AB4">
-        <f>('Formula (ppm)'!AB4*(400435-(85475*'Formula (ppm)'!BH4)))/'Formula (ppm)'!$AI4</f>
-        <v>2.9306980499460802</v>
+        <f>('Formula (ppm)'!AB5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>3.7661093978171641E-2</v>
       </c>
       <c r="AC4">
-        <f>('Formula (ppm)'!AC4*(400435-(85475*'Formula (ppm)'!BI4)))/'Formula (ppm)'!$AI4</f>
-        <v>0.39075973999281066</v>
+        <f>('Formula (ppm)'!AC5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.15064437591268656</v>
       </c>
       <c r="AD4">
-        <f>('Formula (ppm)'!AD4*(400435-(85475*'Formula (ppm)'!BJ4)))/'Formula (ppm)'!$AI4</f>
-        <v>2.0270661512127055</v>
+        <f>('Formula (ppm)'!AD5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <f>('Formula (ppm)'!AE4*(400435-(85475*'Formula (ppm)'!BK4)))/'Formula (ppm)'!$AI4</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>6.9045338959981342</v>
       </c>
       <c r="AF4">
-        <f>('Formula (ppm)'!AF4*(400435-(85475*'Formula (ppm)'!BL4)))/'Formula (ppm)'!$AI4</f>
-        <v>39.491156223023424</v>
-      </c>
-      <c r="AG4">
-        <f>('Formula (ppm)'!AG4*(400435-(85475*'Formula (ppm)'!BM4)))/'Formula (ppm)'!$AI4</f>
-        <v>1.4653490249730401</v>
+        <f>('Formula (ppm)'!AF5*(400435-(85475*'Formula (ppm)'!$AG5)))/'Formula (ppm)'!$AH5</f>
+        <v>0.32639614781082082</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5">
-        <f>('Formula (ppm)'!B5*(400435-(85475*'Formula (ppm)'!AH5)))/'Formula (ppm)'!$AI5</f>
-        <v>7716.4917856476959</v>
+        <f>('Formula (ppm)'!B6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>4648.9947504857691</v>
       </c>
       <c r="C5">
-        <f>('Formula (ppm)'!C5*(400435-(85475*'Formula (ppm)'!AI5)))/'Formula (ppm)'!$AI5</f>
-        <v>-25034.160846883773</v>
+        <f>('Formula (ppm)'!C6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>3322.5411501148355</v>
       </c>
       <c r="D5">
-        <f>('Formula (ppm)'!D5*(400435-(85475*'Formula (ppm)'!AJ5)))/'Formula (ppm)'!$AI5</f>
-        <v>1451.0991561975015</v>
+        <f>('Formula (ppm)'!D6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>2904.492548423274</v>
       </c>
       <c r="E5">
-        <f>('Formula (ppm)'!E5*(400435-(85475*'Formula (ppm)'!AK5)))/'Formula (ppm)'!$AI5</f>
-        <v>384562.45471867494</v>
+        <f>('Formula (ppm)'!E6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>378739.89327093697</v>
       </c>
       <c r="F5">
-        <f>('Formula (ppm)'!F5*(400435-(85475*'Formula (ppm)'!AL5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.41526130072598383</v>
+        <f>('Formula (ppm)'!F6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>30.329216568578754</v>
       </c>
       <c r="G5">
-        <f>('Formula (ppm)'!G5*(400435-(85475*'Formula (ppm)'!AM5)))/'Formula (ppm)'!$AI5</f>
-        <v>2.0385554762911933</v>
+        <f>('Formula (ppm)'!G6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>21.254976570971635</v>
       </c>
       <c r="H5">
-        <f>('Formula (ppm)'!H5*(400435-(85475*'Formula (ppm)'!AN5)))/'Formula (ppm)'!$AI5</f>
-        <v>271.09012731938998</v>
+        <f>('Formula (ppm)'!H6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>3424.4219753131956</v>
       </c>
       <c r="I5">
-        <f>('Formula (ppm)'!I5*(400435-(85475*'Formula (ppm)'!AO5)))/'Formula (ppm)'!$AI5</f>
-        <v>1298.6227567763879</v>
+        <f>('Formula (ppm)'!I6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>4873.8478776336833</v>
       </c>
       <c r="J5">
-        <f>('Formula (ppm)'!J5*(400435-(85475*'Formula (ppm)'!AP5)))/'Formula (ppm)'!$AI5</f>
-        <v>49.139253919241412</v>
+        <f>('Formula (ppm)'!J6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>226.48812534568046</v>
       </c>
       <c r="K5">
-        <f>('Formula (ppm)'!K5*(400435-(85475*'Formula (ppm)'!AQ5)))/'Formula (ppm)'!$AI5</f>
-        <v>93.106617093077389</v>
+        <f>('Formula (ppm)'!K6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>509.77200058629364</v>
       </c>
       <c r="L5">
-        <f>('Formula (ppm)'!L5*(400435-(85475*'Formula (ppm)'!AR5)))/'Formula (ppm)'!$AI5</f>
-        <v>1.5729594724469083</v>
+        <f>('Formula (ppm)'!L6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>1.5123733329345199</v>
       </c>
       <c r="M5">
-        <f>('Formula (ppm)'!M5*(400435-(85475*'Formula (ppm)'!AS5)))/'Formula (ppm)'!$AI5</f>
-        <v>313.2706085325263</v>
+        <f>('Formula (ppm)'!M6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>177.3155545478364</v>
       </c>
       <c r="N5">
-        <f>('Formula (ppm)'!N5*(400435-(85475*'Formula (ppm)'!AT5)))/'Formula (ppm)'!$AI5</f>
-        <v>2.0763065036299189</v>
+        <f>('Formula (ppm)'!N6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>9.1151149525512967</v>
       </c>
       <c r="O5">
-        <f>('Formula (ppm)'!O5*(400435-(85475*'Formula (ppm)'!AU5)))/'Formula (ppm)'!$AI5</f>
-        <v>6.6315971358361656</v>
+        <f>('Formula (ppm)'!O6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>6.2743055839310484</v>
       </c>
       <c r="P5">
-        <f>('Formula (ppm)'!P5*(400435-(85475*'Formula (ppm)'!AV5)))/'Formula (ppm)'!$AI5</f>
-        <v>6.6567644873953169</v>
+        <f>('Formula (ppm)'!P6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <f>('Formula (ppm)'!Q5*(400435-(85475*'Formula (ppm)'!AW5)))/'Formula (ppm)'!$AI5</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>663.03264414948239</v>
       </c>
       <c r="R5">
-        <f>('Formula (ppm)'!R5*(400435-(85475*'Formula (ppm)'!AX5)))/'Formula (ppm)'!$AI5</f>
-        <v>270.95170688581464</v>
+        <f>('Formula (ppm)'!R6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>12.630361077750448</v>
       </c>
       <c r="S5">
-        <f>('Formula (ppm)'!S5*(400435-(85475*'Formula (ppm)'!AY5)))/'Formula (ppm)'!$AI5</f>
-        <v>3.7373517065338544</v>
+        <f>('Formula (ppm)'!S6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>74.2493556560961</v>
       </c>
       <c r="T5">
-        <f>('Formula (ppm)'!T5*(400435-(85475*'Formula (ppm)'!AZ5)))/'Formula (ppm)'!$AI5</f>
-        <v>32.692389675336543</v>
+        <f>('Formula (ppm)'!T6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>2.5138097290668373</v>
       </c>
       <c r="U5">
-        <f>('Formula (ppm)'!U5*(400435-(85475*'Formula (ppm)'!BA5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.64176746475833857</v>
+        <f>('Formula (ppm)'!U6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>10.320926123404496</v>
       </c>
       <c r="V5">
-        <f>('Formula (ppm)'!V5*(400435-(85475*'Formula (ppm)'!BB5)))/'Formula (ppm)'!$AI5</f>
-        <v>2.7306576441678323</v>
+        <f>('Formula (ppm)'!V6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>2.0437477472088106</v>
       </c>
       <c r="W5">
-        <f>('Formula (ppm)'!W5*(400435-(85475*'Formula (ppm)'!BC5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.47817967962386015</v>
+        <f>('Formula (ppm)'!W6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0.57224936921846703</v>
       </c>
       <c r="X5">
-        <f>('Formula (ppm)'!X5*(400435-(85475*'Formula (ppm)'!BD5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.15100410935490322</v>
+        <f>('Formula (ppm)'!X6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>2.2685599994017798</v>
       </c>
       <c r="Y5">
-        <f>('Formula (ppm)'!Y5*(400435-(85475*'Formula (ppm)'!BE5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.49076335540343541</v>
+        <f>('Formula (ppm)'!Y6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>1.6758731527112249</v>
       </c>
       <c r="Z5">
-        <f>('Formula (ppm)'!Z5*(400435-(85475*'Formula (ppm)'!BF5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.35234292182810745</v>
+        <f>('Formula (ppm)'!Z6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0.34743711702549784</v>
       </c>
       <c r="AA5">
-        <f>('Formula (ppm)'!AA5*(400435-(85475*'Formula (ppm)'!BG5)))/'Formula (ppm)'!$AI5</f>
-        <v>6.291837889787634E-2</v>
+        <f>('Formula (ppm)'!AA6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0.83793657635561247</v>
       </c>
       <c r="AB5">
-        <f>('Formula (ppm)'!AB5*(400435-(85475*'Formula (ppm)'!BH5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.25167351559150536</v>
+        <f>('Formula (ppm)'!AB6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0.10218738736044054</v>
       </c>
       <c r="AC5">
-        <f>('Formula (ppm)'!AC5*(400435-(85475*'Formula (ppm)'!BI5)))/'Formula (ppm)'!$AI5</f>
-        <v>3.7751027338725804E-2</v>
+        <f>('Formula (ppm)'!AC6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0.71531171152308382</v>
       </c>
       <c r="AD5">
-        <f>('Formula (ppm)'!AD5*(400435-(85475*'Formula (ppm)'!BJ5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.15100410935490322</v>
+        <f>('Formula (ppm)'!AD6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <f>('Formula (ppm)'!AE5*(400435-(85475*'Formula (ppm)'!BK5)))/'Formula (ppm)'!$AI5</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>16.595231707335543</v>
       </c>
       <c r="AF5">
-        <f>('Formula (ppm)'!AF5*(400435-(85475*'Formula (ppm)'!BL5)))/'Formula (ppm)'!$AI5</f>
-        <v>6.9210216787663974</v>
-      </c>
-      <c r="AG5">
-        <f>('Formula (ppm)'!AG5*(400435-(85475*'Formula (ppm)'!BM5)))/'Formula (ppm)'!$AI5</f>
-        <v>0.32717557026895688</v>
+        <f>('Formula (ppm)'!AF6*(400435-(85475*'Formula (ppm)'!$AG6)))/'Formula (ppm)'!$AH6</f>
+        <v>1.0014363961323174</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6">
-        <f>('Formula (ppm)'!B6*(400435-(85475*'Formula (ppm)'!AH6)))/'Formula (ppm)'!$AI6</f>
-        <v>4648.9184431611575</v>
+        <f>('Formula (ppm)'!B7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>6628.7208018840856</v>
       </c>
       <c r="C6">
-        <f>('Formula (ppm)'!C6*(400435-(85475*'Formula (ppm)'!AI6)))/'Formula (ppm)'!$AI6</f>
-        <v>-10567.036373140776</v>
+        <f>('Formula (ppm)'!C7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>4921.954439985926</v>
       </c>
       <c r="D6">
-        <f>('Formula (ppm)'!D6*(400435-(85475*'Formula (ppm)'!AJ6)))/'Formula (ppm)'!$AI6</f>
-        <v>2909.8938338745866</v>
+        <f>('Formula (ppm)'!D7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>1716.1416828247363</v>
       </c>
       <c r="E6">
-        <f>('Formula (ppm)'!E6*(400435-(85475*'Formula (ppm)'!AK6)))/'Formula (ppm)'!$AI6</f>
-        <v>379444.20985679509</v>
+        <f>('Formula (ppm)'!E7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>379971.78394984739</v>
       </c>
       <c r="F6">
-        <f>('Formula (ppm)'!F6*(400435-(85475*'Formula (ppm)'!AL6)))/'Formula (ppm)'!$AI6</f>
-        <v>30.385617731078032</v>
+        <f>('Formula (ppm)'!F7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>20.824152451571035</v>
       </c>
       <c r="G6">
-        <f>('Formula (ppm)'!G6*(400435-(85475*'Formula (ppm)'!AM6)))/'Formula (ppm)'!$AI6</f>
-        <v>21.294502992130159</v>
+        <f>('Formula (ppm)'!G7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>14.794434515074595</v>
       </c>
       <c r="H6">
-        <f>('Formula (ppm)'!H6*(400435-(85475*'Formula (ppm)'!AN6)))/'Formula (ppm)'!$AI6</f>
-        <v>3430.7901378359238</v>
+        <f>('Formula (ppm)'!H7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>1012.2675206681522</v>
       </c>
       <c r="I6">
-        <f>('Formula (ppm)'!I6*(400435-(85475*'Formula (ppm)'!AO6)))/'Formula (ppm)'!$AI6</f>
-        <v>4882.9114380300298</v>
+        <f>('Formula (ppm)'!I7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>3508.8378857799271</v>
       </c>
       <c r="J6">
-        <f>('Formula (ppm)'!J6*(400435-(85475*'Formula (ppm)'!AP6)))/'Formula (ppm)'!$AI6</f>
-        <v>226.90930976806385</v>
+        <f>('Formula (ppm)'!J7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>226.05081799903317</v>
       </c>
       <c r="K6">
-        <f>('Formula (ppm)'!K6*(400435-(85475*'Formula (ppm)'!AQ6)))/'Formula (ppm)'!$AI6</f>
-        <v>510.71998858913702</v>
+        <f>('Formula (ppm)'!K7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>299.768572096073</v>
       </c>
       <c r="L6">
-        <f>('Formula (ppm)'!L6*(400435-(85475*'Formula (ppm)'!AR6)))/'Formula (ppm)'!$AI6</f>
-        <v>1.5151857898246457</v>
+        <f>('Formula (ppm)'!L7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>2.7477195659983771</v>
       </c>
       <c r="M6">
-        <f>('Formula (ppm)'!M6*(400435-(85475*'Formula (ppm)'!AS6)))/'Formula (ppm)'!$AI6</f>
-        <v>177.64529611511657</v>
+        <f>('Formula (ppm)'!M7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>266.97403023892565</v>
       </c>
       <c r="N6">
-        <f>('Formula (ppm)'!N6*(400435-(85475*'Formula (ppm)'!AT6)))/'Formula (ppm)'!$AI6</f>
-        <v>9.1320657062404322</v>
+        <f>('Formula (ppm)'!N7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>16.320945385073696</v>
       </c>
       <c r="O6">
-        <f>('Formula (ppm)'!O6*(400435-(85475*'Formula (ppm)'!AU6)))/'Formula (ppm)'!$AI6</f>
-        <v>6.2859734794076516</v>
+        <f>('Formula (ppm)'!O7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>5.7498576103299381</v>
       </c>
       <c r="P6">
-        <f>('Formula (ppm)'!P6*(400435-(85475*'Formula (ppm)'!AV6)))/'Formula (ppm)'!$AI6</f>
-        <v>6.5726302504555587</v>
+        <f>('Formula (ppm)'!P7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f>('Formula (ppm)'!Q6*(400435-(85475*'Formula (ppm)'!AW6)))/'Formula (ppm)'!$AI6</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>508.58253818803291</v>
       </c>
       <c r="R6">
-        <f>('Formula (ppm)'!R6*(400435-(85475*'Formula (ppm)'!AX6)))/'Formula (ppm)'!$AI6</f>
-        <v>664.26564045258317</v>
+        <f>('Formula (ppm)'!R7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>15.748503808824031</v>
       </c>
       <c r="S6">
-        <f>('Formula (ppm)'!S6*(400435-(85475*'Formula (ppm)'!AY6)))/'Formula (ppm)'!$AI6</f>
-        <v>12.653848893400419</v>
+        <f>('Formula (ppm)'!S7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>82.380703284284678</v>
       </c>
       <c r="T6">
-        <f>('Formula (ppm)'!T6*(400435-(85475*'Formula (ppm)'!AZ6)))/'Formula (ppm)'!$AI6</f>
-        <v>74.387432086931597</v>
+        <f>('Formula (ppm)'!T7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>3.2692774465814027</v>
       </c>
       <c r="U6">
-        <f>('Formula (ppm)'!U6*(400435-(85475*'Formula (ppm)'!BA6)))/'Formula (ppm)'!$AI6</f>
-        <v>2.5184844884923168</v>
+        <f>('Formula (ppm)'!U7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>13.789481525658525</v>
       </c>
       <c r="V6">
-        <f>('Formula (ppm)'!V6*(400435-(85475*'Formula (ppm)'!BB6)))/'Formula (ppm)'!$AI6</f>
-        <v>10.340119241370894</v>
+        <f>('Formula (ppm)'!V7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>2.8749288051649691</v>
       </c>
       <c r="W6">
-        <f>('Formula (ppm)'!W6*(400435-(85475*'Formula (ppm)'!BC6)))/'Formula (ppm)'!$AI6</f>
-        <v>2.0475483646278998</v>
+        <f>('Formula (ppm)'!W7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>0.80141820674952668</v>
       </c>
       <c r="X6">
-        <f>('Formula (ppm)'!X6*(400435-(85475*'Formula (ppm)'!BD6)))/'Formula (ppm)'!$AI6</f>
-        <v>0.57331354209581187</v>
+        <f>('Formula (ppm)'!X7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>4.4268815229973857</v>
       </c>
       <c r="Y6">
-        <f>('Formula (ppm)'!Y6*(400435-(85475*'Formula (ppm)'!BE6)))/'Formula (ppm)'!$AI6</f>
-        <v>2.2727786847369686</v>
+        <f>('Formula (ppm)'!Y7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>2.5823475550818085</v>
       </c>
       <c r="Z6">
-        <f>('Formula (ppm)'!Z6*(400435-(85475*'Formula (ppm)'!BF6)))/'Formula (ppm)'!$AI6</f>
-        <v>1.6789896589948778</v>
+        <f>('Formula (ppm)'!Z7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>0.53427880449968457</v>
       </c>
       <c r="AA6">
-        <f>('Formula (ppm)'!AA6*(400435-(85475*'Formula (ppm)'!BG6)))/'Formula (ppm)'!$AI6</f>
-        <v>0.34808322198674291</v>
+        <f>('Formula (ppm)'!AA7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>1.5646736417490759</v>
       </c>
       <c r="AB6">
-        <f>('Formula (ppm)'!AB6*(400435-(85475*'Formula (ppm)'!BH6)))/'Formula (ppm)'!$AI6</f>
-        <v>0.83949482949743892</v>
+        <f>('Formula (ppm)'!AB7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>0.22897663049986472</v>
       </c>
       <c r="AC6">
-        <f>('Formula (ppm)'!AC6*(400435-(85475*'Formula (ppm)'!BI6)))/'Formula (ppm)'!$AI6</f>
-        <v>0.102377418231395</v>
+        <f>('Formula (ppm)'!AC7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>1.335697011249211</v>
       </c>
       <c r="AD6">
-        <f>('Formula (ppm)'!AD6*(400435-(85475*'Formula (ppm)'!BJ6)))/'Formula (ppm)'!$AI6</f>
-        <v>0.71664192761976497</v>
+        <f>('Formula (ppm)'!AD7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <f>('Formula (ppm)'!AE6*(400435-(85475*'Formula (ppm)'!BK6)))/'Formula (ppm)'!$AI6</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>75.104334803955638</v>
       </c>
       <c r="AF6">
-        <f>('Formula (ppm)'!AF6*(400435-(85475*'Formula (ppm)'!BL6)))/'Formula (ppm)'!$AI6</f>
-        <v>16.626092720778544</v>
-      </c>
-      <c r="AG6">
-        <f>('Formula (ppm)'!AG6*(400435-(85475*'Formula (ppm)'!BM6)))/'Formula (ppm)'!$AI6</f>
-        <v>1.0032986986676711</v>
+        <f>('Formula (ppm)'!AF7*(400435-(85475*'Formula (ppm)'!$AG7)))/'Formula (ppm)'!$AH7</f>
+        <v>1.6409991852490307</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7">
-        <f>('Formula (ppm)'!B7*(400435-(85475*'Formula (ppm)'!AH7)))/'Formula (ppm)'!$AI7</f>
-        <v>6628.6251462027076</v>
+        <f>('Formula (ppm)'!B8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>8202.0356430626543</v>
       </c>
       <c r="C7">
-        <f>('Formula (ppm)'!C7*(400435-(85475*'Formula (ppm)'!AI7)))/'Formula (ppm)'!$AI7</f>
-        <v>-28136.285952523798</v>
+        <f>('Formula (ppm)'!C8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>4592.5398643382832</v>
       </c>
       <c r="D7">
-        <f>('Formula (ppm)'!D7*(400435-(85475*'Formula (ppm)'!AJ7)))/'Formula (ppm)'!$AI7</f>
-        <v>1720.8751178808473</v>
+        <f>('Formula (ppm)'!D8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>3554.334011095671</v>
       </c>
       <c r="E7">
-        <f>('Formula (ppm)'!E7*(400435-(85475*'Formula (ppm)'!AK7)))/'Formula (ppm)'!$AI7</f>
-        <v>381019.81616098789</v>
+        <f>('Formula (ppm)'!E8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>365495.44680805359</v>
       </c>
       <c r="F7">
-        <f>('Formula (ppm)'!F7*(400435-(85475*'Formula (ppm)'!AL7)))/'Formula (ppm)'!$AI7</f>
-        <v>20.88158930204472</v>
+        <f>('Formula (ppm)'!F8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>6.3968144468019386</v>
       </c>
       <c r="G7">
-        <f>('Formula (ppm)'!G7*(400435-(85475*'Formula (ppm)'!AM7)))/'Formula (ppm)'!$AI7</f>
-        <v>14.835240292167384</v>
+        <f>('Formula (ppm)'!G8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>1.2621517294138354</v>
       </c>
       <c r="H7">
-        <f>('Formula (ppm)'!H7*(400435-(85475*'Formula (ppm)'!AN7)))/'Formula (ppm)'!$AI7</f>
-        <v>1015.0595410569388</v>
+        <f>('Formula (ppm)'!H8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>2282.9169405772741</v>
       </c>
       <c r="I7">
-        <f>('Formula (ppm)'!I7*(400435-(85475*'Formula (ppm)'!AO7)))/'Formula (ppm)'!$AI7</f>
-        <v>3518.5159073681111</v>
+        <f>('Formula (ppm)'!I8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>10558.18606921251</v>
       </c>
       <c r="J7">
-        <f>('Formula (ppm)'!J7*(400435-(85475*'Formula (ppm)'!AP7)))/'Formula (ppm)'!$AI7</f>
-        <v>226.67430781755326</v>
+        <f>('Formula (ppm)'!J8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>548.69177909608732</v>
       </c>
       <c r="K7">
-        <f>('Formula (ppm)'!K7*(400435-(85475*'Formula (ppm)'!AQ7)))/'Formula (ppm)'!$AI7</f>
-        <v>300.59538906700294</v>
+        <f>('Formula (ppm)'!K8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>1263.2417695437834</v>
       </c>
       <c r="L7">
-        <f>('Formula (ppm)'!L7*(400435-(85475*'Formula (ppm)'!AR7)))/'Formula (ppm)'!$AI7</f>
-        <v>2.7552982829820767</v>
+        <f>('Formula (ppm)'!L8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>2.8398413911811295</v>
       </c>
       <c r="M7">
-        <f>('Formula (ppm)'!M7*(400435-(85475*'Formula (ppm)'!AS7)))/'Formula (ppm)'!$AI7</f>
-        <v>267.71039381918905</v>
+        <f>('Formula (ppm)'!M8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>269.06780049776768</v>
       </c>
       <c r="N7">
-        <f>('Formula (ppm)'!N7*(400435-(85475*'Formula (ppm)'!AT7)))/'Formula (ppm)'!$AI7</f>
-        <v>16.365961560490756</v>
+        <f>('Formula (ppm)'!N8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>4.3888457863708368</v>
       </c>
       <c r="O7">
-        <f>('Formula (ppm)'!O7*(400435-(85475*'Formula (ppm)'!AU7)))/'Formula (ppm)'!$AI7</f>
-        <v>5.7657167773513827</v>
+        <f>('Formula (ppm)'!O8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>2.0366539270086883</v>
       </c>
       <c r="P7">
-        <f>('Formula (ppm)'!P7*(400435-(85475*'Formula (ppm)'!AV7)))/'Formula (ppm)'!$AI7</f>
-        <v>5.7784727879207436</v>
+        <f>('Formula (ppm)'!P8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <f>('Formula (ppm)'!Q7*(400435-(85475*'Formula (ppm)'!AW7)))/'Formula (ppm)'!$AI7</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>2526.999873885964</v>
       </c>
       <c r="R7">
-        <f>('Formula (ppm)'!R7*(400435-(85475*'Formula (ppm)'!AX7)))/'Formula (ppm)'!$AI7</f>
-        <v>509.98530256307129</v>
+        <f>('Formula (ppm)'!R8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>6.1386470476036541</v>
       </c>
       <c r="S7">
-        <f>('Formula (ppm)'!S7*(400435-(85475*'Formula (ppm)'!AY7)))/'Formula (ppm)'!$AI7</f>
-        <v>15.791941084869494</v>
+        <f>('Formula (ppm)'!S8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>8.7490063061640857</v>
       </c>
       <c r="T7">
-        <f>('Formula (ppm)'!T7*(400435-(85475*'Formula (ppm)'!AZ7)))/'Formula (ppm)'!$AI7</f>
-        <v>82.607924447184843</v>
+        <f>('Formula (ppm)'!T8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>1.2908369959914223</v>
       </c>
       <c r="U7">
-        <f>('Formula (ppm)'!U7*(400435-(85475*'Formula (ppm)'!BA7)))/'Formula (ppm)'!$AI7</f>
-        <v>3.2782947163258971</v>
+        <f>('Formula (ppm)'!U8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>5.1920332505432771</v>
       </c>
       <c r="V7">
-        <f>('Formula (ppm)'!V7*(400435-(85475*'Formula (ppm)'!BB7)))/'Formula (ppm)'!$AI7</f>
-        <v>13.827515457187829</v>
+        <f>('Formula (ppm)'!V8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>1.1187253965258996</v>
       </c>
       <c r="W7">
-        <f>('Formula (ppm)'!W7*(400435-(85475*'Formula (ppm)'!BC7)))/'Formula (ppm)'!$AI7</f>
-        <v>2.8828583886756913</v>
+        <f>('Formula (ppm)'!W8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.86055799732761495</v>
       </c>
       <c r="X7">
-        <f>('Formula (ppm)'!X7*(400435-(85475*'Formula (ppm)'!BD7)))/'Formula (ppm)'!$AI7</f>
-        <v>0.80362866586977233</v>
+        <f>('Formula (ppm)'!X8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.54502006497415623</v>
       </c>
       <c r="Y7">
-        <f>('Formula (ppm)'!Y7*(400435-(85475*'Formula (ppm)'!BE7)))/'Formula (ppm)'!$AI7</f>
-        <v>4.4390916781377898</v>
+        <f>('Formula (ppm)'!Y8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.65976113128450475</v>
       </c>
       <c r="Z7">
-        <f>('Formula (ppm)'!Z7*(400435-(85475*'Formula (ppm)'!BF7)))/'Formula (ppm)'!$AI7</f>
-        <v>2.5894701455803775</v>
+        <f>('Formula (ppm)'!Z8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.17211159946552299</v>
       </c>
       <c r="AA7">
-        <f>('Formula (ppm)'!AA7*(400435-(85475*'Formula (ppm)'!BG7)))/'Formula (ppm)'!$AI7</f>
-        <v>0.53575244391318166</v>
+        <f>('Formula (ppm)'!AA8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.40159373208622035</v>
       </c>
       <c r="AB7">
-        <f>('Formula (ppm)'!AB7*(400435-(85475*'Formula (ppm)'!BH7)))/'Formula (ppm)'!$AI7</f>
-        <v>1.5689893000314603</v>
+        <f>('Formula (ppm)'!AB8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>5.7370533155174333E-2</v>
       </c>
       <c r="AC7">
-        <f>('Formula (ppm)'!AC7*(400435-(85475*'Formula (ppm)'!BI7)))/'Formula (ppm)'!$AI7</f>
-        <v>0.22960819024850634</v>
+        <f>('Formula (ppm)'!AC8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0.34422319893104597</v>
       </c>
       <c r="AD7">
-        <f>('Formula (ppm)'!AD7*(400435-(85475*'Formula (ppm)'!BJ7)))/'Formula (ppm)'!$AI7</f>
-        <v>1.3393811097829538</v>
+        <f>('Formula (ppm)'!AD8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <f>('Formula (ppm)'!AE7*(400435-(85475*'Formula (ppm)'!BK7)))/'Formula (ppm)'!$AI7</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>22.345822663940403</v>
       </c>
       <c r="AF7">
-        <f>('Formula (ppm)'!AF7*(400435-(85475*'Formula (ppm)'!BL7)))/'Formula (ppm)'!$AI7</f>
-        <v>75.311486401510095</v>
-      </c>
-      <c r="AG7">
-        <f>('Formula (ppm)'!AG7*(400435-(85475*'Formula (ppm)'!BM7)))/'Formula (ppm)'!$AI7</f>
-        <v>1.645525363447629</v>
+        <f>('Formula (ppm)'!AF8*(400435-(85475*'Formula (ppm)'!$AG8)))/'Formula (ppm)'!$AH8</f>
+        <v>2.7251003248707808</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B8">
-        <f>('Formula (ppm)'!B8*(400435-(85475*'Formula (ppm)'!AH8)))/'Formula (ppm)'!$AI8</f>
-        <v>8201.9961712001295</v>
+        <f>('Formula (ppm)'!B9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>6493.1854892619194</v>
       </c>
       <c r="C8">
-        <f>('Formula (ppm)'!C8*(400435-(85475*'Formula (ppm)'!AI8)))/'Formula (ppm)'!$AI8</f>
-        <v>-9079.7644065212844</v>
+        <f>('Formula (ppm)'!C9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>4044.4194934984253</v>
       </c>
       <c r="D8">
-        <f>('Formula (ppm)'!D8*(400435-(85475*'Formula (ppm)'!AJ8)))/'Formula (ppm)'!$AI8</f>
-        <v>3563.8756446434481</v>
+        <f>('Formula (ppm)'!D9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>4667.167349571615</v>
       </c>
       <c r="E8">
-        <f>('Formula (ppm)'!E8*(400435-(85475*'Formula (ppm)'!AK8)))/'Formula (ppm)'!$AI8</f>
-        <v>366476.6217921538</v>
+        <f>('Formula (ppm)'!E9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>297133.94276823453</v>
       </c>
       <c r="F8">
-        <f>('Formula (ppm)'!F8*(400435-(85475*'Formula (ppm)'!AL8)))/'Formula (ppm)'!$AI8</f>
-        <v>6.4139867381887283</v>
+        <f>('Formula (ppm)'!F9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>6.7948965449391521</v>
       </c>
       <c r="G8">
-        <f>('Formula (ppm)'!G8*(400435-(85475*'Formula (ppm)'!AM8)))/'Formula (ppm)'!$AI8</f>
-        <v>1.26553998421661</v>
+        <f>('Formula (ppm)'!G9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>4.6328840079130575</v>
       </c>
       <c r="H8">
-        <f>('Formula (ppm)'!H8*(400435-(85475*'Formula (ppm)'!AN8)))/'Formula (ppm)'!$AI8</f>
-        <v>2289.0454464517934</v>
+        <f>('Formula (ppm)'!H9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>9431.184036261031</v>
       </c>
       <c r="I8">
-        <f>('Formula (ppm)'!I8*(400435-(85475*'Formula (ppm)'!AO8)))/'Formula (ppm)'!$AI8</f>
-        <v>10586.529590695629</v>
+        <f>('Formula (ppm)'!I9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>46989.003988905773</v>
       </c>
       <c r="J8">
-        <f>('Formula (ppm)'!J8*(400435-(85475*'Formula (ppm)'!AP8)))/'Formula (ppm)'!$AI8</f>
-        <v>550.16474586580262</v>
+        <f>('Formula (ppm)'!J9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>275.5462917087338</v>
       </c>
       <c r="K8">
-        <f>('Formula (ppm)'!K8*(400435-(85475*'Formula (ppm)'!AQ8)))/'Formula (ppm)'!$AI8</f>
-        <v>1266.6329505666151</v>
+        <f>('Formula (ppm)'!K9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>2909.8041386080981</v>
       </c>
       <c r="L8">
-        <f>('Formula (ppm)'!L8*(400435-(85475*'Formula (ppm)'!AR8)))/'Formula (ppm)'!$AI8</f>
-        <v>2.8474649644873726</v>
+        <f>('Formula (ppm)'!L9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>1.5442946693043529</v>
       </c>
       <c r="M8">
-        <f>('Formula (ppm)'!M8*(400435-(85475*'Formula (ppm)'!AS8)))/'Formula (ppm)'!$AI8</f>
-        <v>269.79011481708648</v>
+        <f>('Formula (ppm)'!M9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>881.70401076311089</v>
       </c>
       <c r="N8">
-        <f>('Formula (ppm)'!N8*(400435-(85475*'Formula (ppm)'!AT8)))/'Formula (ppm)'!$AI8</f>
-        <v>4.4006276723895761</v>
+        <f>('Formula (ppm)'!N9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>3.4856936821441105</v>
       </c>
       <c r="O8">
-        <f>('Formula (ppm)'!O8*(400435-(85475*'Formula (ppm)'!AU8)))/'Formula (ppm)'!$AI8</f>
-        <v>2.0421213381677115</v>
+        <f>('Formula (ppm)'!O9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>3.1768347482832393</v>
       </c>
       <c r="P8">
-        <f>('Formula (ppm)'!P8*(400435-(85475*'Formula (ppm)'!AV8)))/'Formula (ppm)'!$AI8</f>
-        <v>1.9270722486934746</v>
+        <f>('Formula (ppm)'!P9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <f>('Formula (ppm)'!Q8*(400435-(85475*'Formula (ppm)'!AW8)))/'Formula (ppm)'!$AI8</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!Q9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>26362.389563465586</v>
       </c>
       <c r="R8">
-        <f>('Formula (ppm)'!R8*(400435-(85475*'Formula (ppm)'!AX8)))/'Formula (ppm)'!$AI8</f>
-        <v>2533.7836220358645</v>
+        <f>('Formula (ppm)'!R9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>5.5594608094956701</v>
       </c>
       <c r="S8">
-        <f>('Formula (ppm)'!S8*(400435-(85475*'Formula (ppm)'!AY8)))/'Formula (ppm)'!$AI8</f>
-        <v>6.1551262868716945</v>
+        <f>('Formula (ppm)'!S9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>9.7069950641987877</v>
       </c>
       <c r="T8">
-        <f>('Formula (ppm)'!T8*(400435-(85475*'Formula (ppm)'!AZ8)))/'Formula (ppm)'!$AI8</f>
-        <v>8.7724930724105921</v>
+        <f>('Formula (ppm)'!T9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>1.1030676209316805</v>
       </c>
       <c r="U8">
-        <f>('Formula (ppm)'!U8*(400435-(85475*'Formula (ppm)'!BA8)))/'Formula (ppm)'!$AI8</f>
-        <v>1.2943022565851694</v>
+        <f>('Formula (ppm)'!U9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>4.6328840079130575</v>
       </c>
       <c r="V8">
-        <f>('Formula (ppm)'!V8*(400435-(85475*'Formula (ppm)'!BB8)))/'Formula (ppm)'!$AI8</f>
-        <v>5.2059712987092359</v>
+        <f>('Formula (ppm)'!V9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0.88245409674534447</v>
       </c>
       <c r="W8">
-        <f>('Formula (ppm)'!W8*(400435-(85475*'Formula (ppm)'!BC8)))/'Formula (ppm)'!$AI8</f>
-        <v>1.1217286223738134</v>
+        <f>('Formula (ppm)'!W9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>6.9272646594509535</v>
       </c>
       <c r="X8">
-        <f>('Formula (ppm)'!X8*(400435-(85475*'Formula (ppm)'!BD8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.8628681710567796</v>
+        <f>('Formula (ppm)'!X9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>1.0148222112571461</v>
       </c>
       <c r="Y8">
-        <f>('Formula (ppm)'!Y8*(400435-(85475*'Formula (ppm)'!BE8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.54648317500262711</v>
+        <f>('Formula (ppm)'!Y9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0.57359516288447387</v>
       </c>
       <c r="Z8">
-        <f>('Formula (ppm)'!Z8*(400435-(85475*'Formula (ppm)'!BF8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.66153226447686442</v>
+        <f>('Formula (ppm)'!Z9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0.13236811451180167</v>
       </c>
       <c r="AA8">
-        <f>('Formula (ppm)'!AA8*(400435-(85475*'Formula (ppm)'!BG8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.17257363421135594</v>
+        <f>('Formula (ppm)'!AA9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0.44122704837267224</v>
       </c>
       <c r="AB8">
-        <f>('Formula (ppm)'!AB8*(400435-(85475*'Formula (ppm)'!BH8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.40267181315983047</v>
+        <f>('Formula (ppm)'!AB9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>4.412270483726722E-2</v>
       </c>
       <c r="AC8">
-        <f>('Formula (ppm)'!AC8*(400435-(85475*'Formula (ppm)'!BI8)))/'Formula (ppm)'!$AI8</f>
-        <v>5.7524544737118641E-2</v>
+        <f>('Formula (ppm)'!AC9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0.30885893386087054</v>
       </c>
       <c r="AD8">
-        <f>('Formula (ppm)'!AD8*(400435-(85475*'Formula (ppm)'!BJ8)))/'Formula (ppm)'!$AI8</f>
-        <v>0.34514726842271187</v>
+        <f>('Formula (ppm)'!AD9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <f>('Formula (ppm)'!AE8*(400435-(85475*'Formula (ppm)'!BK8)))/'Formula (ppm)'!$AI8</f>
-        <v>0</v>
+        <f>('Formula (ppm)'!AE9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>29.871071174829908</v>
       </c>
       <c r="AF8">
-        <f>('Formula (ppm)'!AF8*(400435-(85475*'Formula (ppm)'!BL8)))/'Formula (ppm)'!$AI8</f>
-        <v>22.405810175107714</v>
-      </c>
-      <c r="AG8">
-        <f>('Formula (ppm)'!AG8*(400435-(85475*'Formula (ppm)'!BM8)))/'Formula (ppm)'!$AI8</f>
-        <v>2.7324158750131353</v>
+        <f>('Formula (ppm)'!AF9*(400435-(85475*'Formula (ppm)'!$AG9)))/'Formula (ppm)'!$AH9</f>
+        <v>2.3826260612124295</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B9">
-        <f>('Formula (ppm)'!B9*(400435-(85475*'Formula (ppm)'!AH9)))/'Formula (ppm)'!$AI9</f>
-        <v>6493.1323910708097</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f>('Formula (ppm)'!C9*(400435-(85475*'Formula (ppm)'!AI9)))/'Formula (ppm)'!$AI9</f>
-        <v>-3778.7235668279095</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f>('Formula (ppm)'!D9*(400435-(85475*'Formula (ppm)'!AJ9)))/'Formula (ppm)'!$AI9</f>
-        <v>4680.7287319133038</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <f>('Formula (ppm)'!E9*(400435-(85475*'Formula (ppm)'!AK9)))/'Formula (ppm)'!$AI9</f>
-        <v>297997.32449482789</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <f>('Formula (ppm)'!F9*(400435-(85475*'Formula (ppm)'!AL9)))/'Formula (ppm)'!$AI9</f>
-        <v>6.8146404673478047</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <f>('Formula (ppm)'!G9*(400435-(85475*'Formula (ppm)'!AM9)))/'Formula (ppm)'!$AI9</f>
-        <v>4.6463457731916842</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <f>('Formula (ppm)'!H9*(400435-(85475*'Formula (ppm)'!AN9)))/'Formula (ppm)'!$AI9</f>
-        <v>9458.5882159423745</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <f>('Formula (ppm)'!I9*(400435-(85475*'Formula (ppm)'!AO9)))/'Formula (ppm)'!$AI9</f>
-        <v>47125.539879140597</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <f>('Formula (ppm)'!J9*(400435-(85475*'Formula (ppm)'!AP9)))/'Formula (ppm)'!$AI9</f>
-        <v>276.34694622459114</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <f>('Formula (ppm)'!K9*(400435-(85475*'Formula (ppm)'!AQ9)))/'Formula (ppm)'!$AI9</f>
-        <v>2918.259152861383</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <f>('Formula (ppm)'!L9*(400435-(85475*'Formula (ppm)'!AR9)))/'Formula (ppm)'!$AI9</f>
-        <v>1.5487819243972285</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <f>('Formula (ppm)'!M9*(400435-(85475*'Formula (ppm)'!AS9)))/'Formula (ppm)'!$AI9</f>
-        <v>884.26597700656612</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <f>('Formula (ppm)'!N9*(400435-(85475*'Formula (ppm)'!AT9)))/'Formula (ppm)'!$AI9</f>
-        <v>3.4958220579251722</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <f>('Formula (ppm)'!O9*(400435-(85475*'Formula (ppm)'!AU9)))/'Formula (ppm)'!$AI9</f>
-        <v>3.1860656730457264</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <f>('Formula (ppm)'!P9*(400435-(85475*'Formula (ppm)'!AV9)))/'Formula (ppm)'!$AI9</f>
-        <v>3.2745674972969967</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <f>('Formula (ppm)'!Q9*(400435-(85475*'Formula (ppm)'!AW9)))/'Formula (ppm)'!$AI9</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>('Formula (ppm)'!R9*(400435-(85475*'Formula (ppm)'!AX9)))/'Formula (ppm)'!$AI9</f>
-        <v>26438.990725912336</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <f>('Formula (ppm)'!S9*(400435-(85475*'Formula (ppm)'!AY9)))/'Formula (ppm)'!$AI9</f>
-        <v>5.5756149278300224</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <f>('Formula (ppm)'!T9*(400435-(85475*'Formula (ppm)'!AZ9)))/'Formula (ppm)'!$AI9</f>
-        <v>9.735200667639722</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <f>('Formula (ppm)'!U9*(400435-(85475*'Formula (ppm)'!BA9)))/'Formula (ppm)'!$AI9</f>
-        <v>1.1062728031408775</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <f>('Formula (ppm)'!V9*(400435-(85475*'Formula (ppm)'!BB9)))/'Formula (ppm)'!$AI9</f>
-        <v>4.6463457731916842</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <f>('Formula (ppm)'!W9*(400435-(85475*'Formula (ppm)'!BC9)))/'Formula (ppm)'!$AI9</f>
-        <v>0.885018242512702</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <f>('Formula (ppm)'!X9*(400435-(85475*'Formula (ppm)'!BD9)))/'Formula (ppm)'!$AI9</f>
-        <v>6.947393203724709</v>
+        <v>0</v>
       </c>
       <c r="Y9">
-        <f>('Formula (ppm)'!Y9*(400435-(85475*'Formula (ppm)'!BE9)))/'Formula (ppm)'!$AI9</f>
-        <v>1.0177709788896072</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <f>('Formula (ppm)'!Z9*(400435-(85475*'Formula (ppm)'!BF9)))/'Formula (ppm)'!$AI9</f>
-        <v>0.5752618576332561</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <f>('Formula (ppm)'!AA9*(400435-(85475*'Formula (ppm)'!BG9)))/'Formula (ppm)'!$AI9</f>
-        <v>0.13275273637690529</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <f>('Formula (ppm)'!AB9*(400435-(85475*'Formula (ppm)'!BH9)))/'Formula (ppm)'!$AI9</f>
-        <v>0.442509121256351</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <f>('Formula (ppm)'!AC9*(400435-(85475*'Formula (ppm)'!BI9)))/'Formula (ppm)'!$AI9</f>
-        <v>4.4250912125635096E-2</v>
+        <v>0</v>
       </c>
       <c r="AD9">
-        <f>('Formula (ppm)'!AD9*(400435-(85475*'Formula (ppm)'!BJ9)))/'Formula (ppm)'!$AI9</f>
-        <v>0.30975638487944568</v>
+        <v>0</v>
       </c>
       <c r="AE9">
-        <f>('Formula (ppm)'!AE9*(400435-(85475*'Formula (ppm)'!BK9)))/'Formula (ppm)'!$AI9</f>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f>('Formula (ppm)'!AF9*(400435-(85475*'Formula (ppm)'!BL9)))/'Formula (ppm)'!$AI9</f>
-        <v>29.957867509054964</v>
-      </c>
-      <c r="AG9">
-        <f>('Formula (ppm)'!AG9*(400435-(85475*'Formula (ppm)'!BM9)))/'Formula (ppm)'!$AI9</f>
-        <v>2.3895492547842951</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -17160,110 +17045,6 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
         <v>0</v>
       </c>
     </row>

</xml_diff>